<commit_message>
Added AIC table and more figures
</commit_message>
<xml_diff>
--- a/tables/OSM_all_covariates_summary_formatted.xlsx
+++ b/tables/OSM_all_covariates_summary_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidanbrushett\Desktop\projects\OSM_red_squirrel_distribution\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0792332A-7D9C-4606-A623-22FDB86C5B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9EB31E-BC05-4C8F-8CEF-00AB3000ECFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Covariate</t>
   </si>
@@ -239,13 +239,25 @@
   </si>
   <si>
     <t>Anthro. cohesion</t>
+  </si>
+  <si>
+    <t>750 m</t>
+  </si>
+  <si>
+    <t>3000 m</t>
+  </si>
+  <si>
+    <t>4000 m</t>
+  </si>
+  <si>
+    <t>Scale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +277,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,12 +387,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -681,45 +693,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="80.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="10"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="5"/>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6" t="s">
         <v>49</v>
@@ -727,95 +744,111 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
         <v>50</v>
@@ -823,112 +856,131 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>51</v>
@@ -936,130 +988,152 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="9"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
First draft of paper added
</commit_message>
<xml_diff>
--- a/tables/OSM_all_covariates_summary_formatted.xlsx
+++ b/tables/OSM_all_covariates_summary_formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmya\Documents\GitHub\OSM_red_squirrel_distribution\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidanbrushett\Desktop\projects\OSM_red_squirrel_distribution\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE9D627-057C-4749-B70F-B24CE437ABAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EE9037-2540-494B-9C29-9042EE9D1D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-3315" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="5532" windowWidth="23040" windowHeight="12276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="140">
   <si>
     <t>Covariate</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Sum of the footprint of all anthropogenic disturbances at a site.</t>
+  </si>
+  <si>
+    <t>Median (5%, 95%)</t>
   </si>
 </sst>
 </file>
@@ -965,810 +968,874 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B24:G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="83.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="6"/>
+      <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="6"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="F11" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18" t="s">
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="F12" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="D13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="F15" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="F17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18" t="s">
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="D18" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="F18" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18" t="s">
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="F20" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="F21" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18" t="s">
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="D22" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="E22" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="F22" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18" t="s">
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="D25" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="30" t="s">
+      <c r="E25" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="31" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4" t="s">
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4" t="s">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="26"/>
+      <c r="E28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4" t="s">
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="26"/>
+      <c r="E29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="26"/>
+      <c r="E30" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4" t="s">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="26"/>
+      <c r="E31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4" t="s">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="26"/>
+      <c r="E32" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4" t="s">
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="26"/>
+      <c r="E33" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4" t="s">
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="26"/>
+      <c r="E34" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="31" t="s">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="D35" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4" t="s">
+      <c r="E35" s="34"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="26"/>
+      <c r="E36" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4" t="s">
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="26"/>
+      <c r="E37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4" t="s">
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="26"/>
+      <c r="E38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4" t="s">
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="26"/>
+      <c r="E39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4" t="s">
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="26"/>
+      <c r="E40" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4" t="s">
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="26"/>
+      <c r="E41" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="8" t="s">
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="24" t="s">
+      <c r="D42" s="27"/>
+      <c r="E42" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="F42" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-      <c r="B42" s="31" t="s">
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="D43" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4" t="s">
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="26"/>
+      <c r="E44" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4" t="s">
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="26"/>
+      <c r="E45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4" t="s">
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="26"/>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="26"/>
+      <c r="E46" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4" t="s">
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="3" t="s">
+      <c r="D47" s="26"/>
+      <c r="E47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="28"/>
-      <c r="D47" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="28"/>
+      <c r="E48" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>